<commit_message>
update thống kê + docs
</commit_message>
<xml_diff>
--- a/docs/stats-ModulesView-NativeView.xlsx
+++ b/docs/stats-ModulesView-NativeView.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t xml:space="preserve">STT</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">Layout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Draw</t>
   </si>
   <si>
     <t xml:space="preserve">ModulesView</t>
@@ -104,7 +101,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +118,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF999966"/>
         <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF004586"/>
-        <bgColor rgb="FF333399"/>
       </patternFill>
     </fill>
     <fill>
@@ -182,7 +173,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,31 +190,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,7 +277,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF999966"/>
-      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -315,19 +298,19 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -342,9 +325,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -353,23 +334,19 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -378,24 +355,20 @@
       <c r="A3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="C3" s="10" t="n">
-        <v>0.053</v>
-      </c>
-      <c r="D3" s="10" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="E3" s="10" t="n">
-        <v>0.062</v>
-      </c>
-      <c r="F3" s="10" t="n">
-        <v>0.593</v>
-      </c>
-      <c r="G3" s="10" t="n">
-        <v>0.538</v>
-      </c>
+      <c r="B3" s="4" t="n">
+        <v>0.02362</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>0.05655</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>0.02565</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0.02049</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -404,24 +377,20 @@
       <c r="A4" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="n">
-        <v>0.154</v>
-      </c>
-      <c r="C4" s="10" t="n">
-        <v>0.067</v>
-      </c>
-      <c r="D4" s="10" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="E4" s="10" t="n">
-        <v>0.066</v>
-      </c>
-      <c r="F4" s="10" t="n">
-        <v>0.597</v>
-      </c>
-      <c r="G4" s="10" t="n">
-        <v>0.681</v>
-      </c>
+      <c r="B4" s="4" t="n">
+        <v>0.04624</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>0.02935</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>0.01237</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>0.03132</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -430,24 +399,20 @@
       <c r="A5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="n">
-        <v>0.102</v>
-      </c>
-      <c r="C5" s="10" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="D5" s="10" t="n">
-        <v>0.054</v>
-      </c>
-      <c r="E5" s="10" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="F5" s="10" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="G5" s="10" t="n">
-        <v>0.572</v>
-      </c>
+      <c r="B5" s="4" t="n">
+        <v>0.04671</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>0.04391</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>0.01043</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0.02526</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -456,24 +421,20 @@
       <c r="A6" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="n">
-        <v>0.115</v>
-      </c>
-      <c r="C6" s="10" t="n">
-        <v>0.063</v>
-      </c>
-      <c r="D6" s="10" t="n">
-        <v>0.054</v>
-      </c>
-      <c r="E6" s="10" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="F6" s="10" t="n">
-        <v>0.333</v>
-      </c>
-      <c r="G6" s="10" t="n">
-        <v>0.529</v>
-      </c>
+      <c r="B6" s="4" t="n">
+        <v>0.04502</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>0.03412</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>0.00976</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>0.02283</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -482,24 +443,20 @@
       <c r="A7" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="n">
-        <v>0.144</v>
-      </c>
-      <c r="C7" s="10" t="n">
-        <v>0.055</v>
-      </c>
-      <c r="D7" s="10" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="E7" s="10" t="n">
-        <v>0.052</v>
-      </c>
-      <c r="F7" s="10" t="n">
-        <v>0.575</v>
-      </c>
-      <c r="G7" s="10" t="n">
-        <v>0.995</v>
-      </c>
+      <c r="B7" s="4" t="n">
+        <v>0.03799</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>0.0331</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>0.01274</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>0.0282</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -508,24 +465,20 @@
       <c r="A8" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="n">
-        <v>0.111</v>
-      </c>
-      <c r="C8" s="10" t="n">
-        <v>0.097</v>
-      </c>
-      <c r="D8" s="10" t="n">
-        <v>0.056</v>
-      </c>
-      <c r="E8" s="10" t="n">
-        <v>0.055</v>
-      </c>
-      <c r="F8" s="10" t="n">
-        <v>0.568</v>
-      </c>
-      <c r="G8" s="10" t="n">
-        <v>0.59</v>
-      </c>
+      <c r="B8" s="4" t="n">
+        <v>0.02407</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>0.06603</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>0.01012</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>0.02544</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -534,24 +487,20 @@
       <c r="A9" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="10" t="n">
-        <v>0.168</v>
-      </c>
-      <c r="C9" s="10" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="D9" s="10" t="n">
-        <v>0.086</v>
-      </c>
-      <c r="E9" s="10" t="n">
-        <v>0.068</v>
-      </c>
-      <c r="F9" s="10" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="G9" s="10" t="n">
-        <v>0.79</v>
-      </c>
+      <c r="B9" s="4" t="n">
+        <v>0.02552</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>0.06917</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>0.0155</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>0.03523</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -560,24 +509,20 @@
       <c r="A10" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="n">
-        <v>0.158</v>
-      </c>
-      <c r="C10" s="10" t="n">
-        <v>0.062</v>
-      </c>
-      <c r="D10" s="10" t="n">
+      <c r="B10" s="4" t="n">
+        <v>0.03425</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>0.04425</v>
+      </c>
+      <c r="D10" s="4" t="n">
         <v>0.069</v>
       </c>
-      <c r="E10" s="10" t="n">
+      <c r="E10" s="4" t="n">
         <v>0.054</v>
       </c>
-      <c r="F10" s="10" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="G10" s="10" t="n">
-        <v>0.713</v>
-      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -586,24 +531,20 @@
       <c r="A11" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="10" t="n">
-        <v>0.138</v>
-      </c>
-      <c r="C11" s="10" t="n">
-        <v>0.074</v>
-      </c>
-      <c r="D11" s="10" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="E11" s="10" t="n">
-        <v>0.061</v>
-      </c>
-      <c r="F11" s="10" t="n">
-        <v>0.483</v>
-      </c>
-      <c r="G11" s="10" t="n">
-        <v>0.548</v>
-      </c>
+      <c r="B11" s="4" t="n">
+        <v>0.05175</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>0.04198</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>0.01551</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>0.03523</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -612,63 +553,52 @@
       <c r="A12" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="10" t="n">
-        <v>0.196</v>
-      </c>
-      <c r="C12" s="10" t="n">
-        <v>0.114</v>
-      </c>
-      <c r="D12" s="10" t="n">
-        <v>0.085</v>
-      </c>
-      <c r="E12" s="10" t="n">
-        <v>0.062</v>
-      </c>
-      <c r="F12" s="10" t="n">
-        <v>0.541</v>
-      </c>
-      <c r="G12" s="10" t="n">
-        <v>0.807</v>
-      </c>
+      <c r="B12" s="4" t="n">
+        <v>0.02661</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>0.03214</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>0.01183</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>0.02873</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="24.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="12" t="n">
+      <c r="A13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="10" t="n">
         <f aca="false">AVERAGE(B3:B12)</f>
-        <v>0.1411</v>
-      </c>
-      <c r="C13" s="12" t="n">
+        <v>0.036178</v>
+      </c>
+      <c r="C13" s="10" t="n">
         <f aca="false">AVERAGE(C3:C12)</f>
-        <v>0.0708</v>
-      </c>
-      <c r="D13" s="12" t="n">
+        <v>0.04506</v>
+      </c>
+      <c r="D13" s="10" t="n">
         <f aca="false">AVERAGE(D3:D12)</f>
-        <v>0.0696</v>
-      </c>
-      <c r="E13" s="12" t="n">
+        <v>0.019291</v>
+      </c>
+      <c r="E13" s="10" t="n">
         <f aca="false">AVERAGE(E3:E12)</f>
-        <v>0.0598</v>
-      </c>
-      <c r="F13" s="12" t="n">
-        <f aca="false">AVERAGE(F3:F12)</f>
-        <v>0.5225</v>
-      </c>
-      <c r="G13" s="12" t="n">
-        <f aca="false">AVERAGE(G3:G12)</f>
-        <v>0.6763</v>
-      </c>
+        <v>0.030673</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>